<commit_message>
Update of data and plots
</commit_message>
<xml_diff>
--- a/data/Dispersivity_GeoStats.xlsx
+++ b/data/Dispersivity_GeoStats.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="180">
   <si>
     <t xml:space="preserve">Site name</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">A_L</t>
   </si>
   <si>
-    <t xml:space="preserve">R – A_L</t>
+    <t xml:space="preserve">Reliability – A_L</t>
   </si>
   <si>
     <t xml:space="preserve">A_T</t>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">A_V</t>
   </si>
   <si>
-    <t xml:space="preserve">R – A_T/A_V</t>
+    <t xml:space="preserve">Reliability – A_T/A_V</t>
   </si>
   <si>
     <t xml:space="preserve">KG </t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Correlation length</t>
   </si>
   <si>
-    <t xml:space="preserve">Porosoty</t>
+    <t xml:space="preserve">Porosity</t>
   </si>
   <si>
     <t xml:space="preserve">Hydraulic gradient</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Flow velocity (average)</t>
   </si>
   <si>
-    <t xml:space="preserve">Aquifer material </t>
+    <t xml:space="preserve">Aquifer material description</t>
   </si>
   <si>
     <t xml:space="preserve">Heterogeneity class</t>
@@ -97,6 +97,9 @@
     <t xml:space="preserve">[m]</t>
   </si>
   <si>
+    <t xml:space="preserve">[1:high, 2:medium]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[1e-3m/s] </t>
   </si>
   <si>
@@ -109,13 +112,13 @@
     <t xml:space="preserve">fairly homogeneous/mildly heterogeneous (intensively studied)</t>
   </si>
   <si>
-    <t xml:space="preserve">Grindsted*</t>
+    <t xml:space="preserve">Grindsted</t>
   </si>
   <si>
     <t xml:space="preserve">glacial outwash plain, sandy</t>
   </si>
   <si>
-    <t xml:space="preserve">Petersen et al., 1998, Bjerg et al., 1992</t>
+    <t xml:space="preserve">Petersen et al., 1998; Bjerg et al., 1992</t>
   </si>
   <si>
     <t xml:space="preserve">Borden</t>
@@ -124,7 +127,7 @@
     <t xml:space="preserve">glaciofluvial/glaciolacustrine sand</t>
   </si>
   <si>
-    <t xml:space="preserve">Freyberg et al., 1986, Rajaram et al., 1991, Rivett et al., 1994, Sudicky et al., 1983,Gelhar et al., 1985, Sykes et al., 1982, Sudicky, 1986</t>
+    <t xml:space="preserve">Freyberg et al., 1986; Sudicky, 1986; Rajaram et al., 1991</t>
   </si>
   <si>
     <t xml:space="preserve">Vejen (Jutland Aquifer)</t>
@@ -133,7 +136,7 @@
     <t xml:space="preserve">layers of fine-grained, medium-grained, and coarse-grained sand in an glacial outwash plain</t>
   </si>
   <si>
-    <t xml:space="preserve">Jensen et al., 1993, Bjerg et al., 1992</t>
+    <t xml:space="preserve">Jensen et al., 1993; Bjerg et al., 1992</t>
   </si>
   <si>
     <t xml:space="preserve">Cape Cod</t>
@@ -142,7 +145,7 @@
     <t xml:space="preserve">medium to coarse sand with some gravel overlying silty sand and till</t>
   </si>
   <si>
-    <t xml:space="preserve">Garabedian et al., 1991, Hess et al., 1992</t>
+    <t xml:space="preserve">Garabedian et al., 1991; Hess et al., 1992</t>
   </si>
   <si>
     <t xml:space="preserve">Chalk River/Twin Lake</t>
@@ -157,138 +160,141 @@
     <t xml:space="preserve">layered/stratified medium sand, glaciofluvial, very fine to medium grained sand and well sorted (0.12-0.21mm)</t>
   </si>
   <si>
-    <t xml:space="preserve">Moltyaner and Killey, 1988, Moltyaner et al., 1993, Pickens and Grisakm 1981, Huyakorn et al., 1986, Dagan et al., 1997</t>
+    <t xml:space="preserve">Moltyaner and Killey, 1988; Moltyaner et al., 1993; Dagan et al., 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderately heterogeneous (intensively studied)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lauswiesen Site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alluvial sands and gravel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haendel and Dietrich, 2012; Mueller et al., 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krauthausen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alluvial deposits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vereecken et al., 2000; Vanderborght et al., 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highly heterogeneous (intensively studied)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horkheimer Insel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6 – 3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poorly sorted alluvial sand and gravel deposits of holocene age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ptak and Teutsch, 1994; Schad, 1997; Zech et al., 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fairly homogeneous/mildly heterogeneous (moderate information)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palo Alto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sand, gravel, and silt, “permeable stratum of silty sand and some gravel”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valocchi et al., 1981; Roberts et al., 1981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burdekin Delta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sand channels with clay lenses, complex sedimentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiebenga et al., 1967; Lenda and Zuber, 1970; McMahon  et al., 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Mexico State University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layers of clay loam and sands, fluvial deposits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kies, 1981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonnaud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alluvial sand layers, fine sand and gravels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauty, 1977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.25-0.35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medium sand, fluvial deposits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huyakorn et al., 1986; Molz et al., 1986, 1988;  Sykes et al., 1982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sjoelund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorted fine-grained sand layer within layered stratum, glacial outwash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prommer et al., 2006; Tuxen et al., 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambridge site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sand with minor silt, “sand plain with glaciolacustrine and outwash sand”, “ moderately permeable fine sand to very permeable coarse sand with coarser material dominating”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robertson et al., 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas Plant Facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandy aquifer, medium coarse sand with interbeds of small gravel and cobbles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiang et al., 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rabis Creek Catchment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2-0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium-grained outwash sand (0.2-0.6 mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engesgaard et al., 1996</t>
   </si>
   <si>
     <t xml:space="preserve">moderately heterogeneous (moderate information)</t>
   </si>
   <si>
-    <t xml:space="preserve">Lauswiesen Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alluvial sands and gravel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haendel and Dietrich, 2012, Mueller et al., 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krauthausen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alluvial deposits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vereeckenv et al., 2000, Vanderborght et al., 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Highly heterogeneous (intensively studied)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horkheimer Insel*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.6 – 3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">poorly sorted alluvial sand and gravel deposits of holocene age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ptak and Teutsch, 1994, Schad, 1997, Zech et al., 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fairly homogeneous/mildly heterogeneous (moderate information)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palo Alto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sand, gravel, and silt, “permeable stratum of silty sand and some gravel”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valocchi et al., 1981, Roberts et al., 1981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burdekin Delta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sand channels with clay lenses, complex sedimentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wiebenga et al., 1967, Lenda and Zuber, 1970, McMahon  et al., 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Mexico State University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layers of clay loam and sands, fluvial deposits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kies, 1981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonnaud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alluvial sand layers, fine sand and gravels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sauty, 1977</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.25-0.35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medium sand, fluvial deposits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huyakorn et al., 1986, Molz et al., 1986, Sykes et al., 1982, Papadopulos et al., 1978, Molz et al., 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sjoelund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sorted fine-grained sand layer within layered stratum, glacial outwash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prommer et al., 2006, Tuxen et al., 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cambridge site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sand with minor silt, “sand plain with glaciolacustrine and outwash sand”, “ moderately permeable fine sand to very permeable coarse sand with coarser material dominating”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robertson et al., 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas Plant Facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sandy aquifer, medium coarse sand with interbeds of small gravel and cobbles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chiang et al., 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rabis Creek Catchment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2-0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medium-grained outwash sand (0.2-0.6 mm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engesgaard et al., 1996</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hebei Province Aquifer</t>
   </si>
   <si>
@@ -316,7 +322,7 @@
     <t xml:space="preserve">Iris, 1980</t>
   </si>
   <si>
-    <t xml:space="preserve">Zeitz*</t>
+    <t xml:space="preserve">Zeitz</t>
   </si>
   <si>
     <t xml:space="preserve">layers of fine to coarse sand and fine gravel, glaciofluvial</t>
@@ -331,7 +337,7 @@
     <t xml:space="preserve">gravel, sand, and silt, poorly sorted, high median grain size</t>
   </si>
   <si>
-    <t xml:space="preserve">Wilson, 1971, Welty and Gelhar, 1989</t>
+    <t xml:space="preserve">Wilson, 1971; Welty and Gelhar, 1989</t>
   </si>
   <si>
     <t xml:space="preserve">Testfeld Sued</t>
@@ -340,7 +346,7 @@
     <t xml:space="preserve">fluvial heterogeneous gravel and sand</t>
   </si>
   <si>
-    <t xml:space="preserve">Boesel et al., 1900, Herfort and Ptak, 2002</t>
+    <t xml:space="preserve">Boesel et al., 2000; Herfort and Ptak, 2002</t>
   </si>
   <si>
     <t xml:space="preserve">Burnham Aquifer</t>
@@ -364,13 +370,13 @@
     <t xml:space="preserve">Naymik and Barcelona, 1981</t>
   </si>
   <si>
-    <t xml:space="preserve">Osterhofen*</t>
+    <t xml:space="preserve">Osterhofen</t>
   </si>
   <si>
     <t xml:space="preserve">gravel aquifer, moraine sediments and periglacial deposits</t>
   </si>
   <si>
-    <t xml:space="preserve">Maier et al., 2006, Ruegner et al., 2006</t>
+    <t xml:space="preserve">Maier et al., 2006; Ruegner et al., 2006</t>
   </si>
   <si>
     <t xml:space="preserve">highly heterogeneous (moderate information)</t>
@@ -382,7 +388,7 @@
     <t xml:space="preserve">heterogeneous alluvial sediments, “layers of pebbly conclomerate and well-sorted sand of variable clay content with non-continuous clay lenses”</t>
   </si>
   <si>
-    <t xml:space="preserve">Broermann et al., 1997, Bassett et al., 1980</t>
+    <t xml:space="preserve">Broermann et al., 1997; Bassett et al., 1980</t>
   </si>
   <si>
     <t xml:space="preserve">Grenoble Aquifer</t>
@@ -412,7 +418,7 @@
     <t xml:space="preserve">layered gravel and silty sand, glaciofluvial outwash deposits, “interbedded and nonuniformly graded fine and coarse layers of sand and gravel”</t>
   </si>
   <si>
-    <t xml:space="preserve">Hoehn and Santschi, 1987, Hufschmied, 1986</t>
+    <t xml:space="preserve">Hoehn and Santschi, 1987; Hufschmied, 1986</t>
   </si>
   <si>
     <t xml:space="preserve">Corbas</t>
@@ -421,7 +427,7 @@
     <t xml:space="preserve">sand and gravel with clay lenses</t>
   </si>
   <si>
-    <t xml:space="preserve">Sauty, 1977, Welty and Gelhar, 1989</t>
+    <t xml:space="preserve">Sauty, 1977; Welty and Gelhar, 1989</t>
   </si>
   <si>
     <t xml:space="preserve">Hanford (shallow)</t>
@@ -430,7 +436,7 @@
     <t xml:space="preserve">glacio-fluviatile sands and gravels, very coarse and permeable</t>
   </si>
   <si>
-    <t xml:space="preserve">Bierschenk et al., 1959, Cole, 1974, Gelhar,1982</t>
+    <t xml:space="preserve">Bierschenk et al., 1959; Cole, 1974; Gelhar,1982</t>
   </si>
   <si>
     <t xml:space="preserve">reliable, but preasymptotic macrodispersivity</t>
@@ -469,7 +475,7 @@
     <t xml:space="preserve">fine to medium uniform sand</t>
   </si>
   <si>
-    <t xml:space="preserve">Palmer and nadon, 1986 (Reanalysis)</t>
+    <t xml:space="preserve">Palmer and Nadon, 1986; Zech et al, 2015 (Reanalysis)</t>
   </si>
   <si>
     <t xml:space="preserve">Byles-Saint Vulbas</t>
@@ -505,7 +511,7 @@
     <t xml:space="preserve">Sand and silt, fluvial deposits</t>
   </si>
   <si>
-    <t xml:space="preserve">Hyndman and Gerelick, 1996 (Reanalysis)</t>
+    <t xml:space="preserve">Hyndman and Gerelick, 1996; Zech et al., 2015 (Reanalysis)</t>
   </si>
   <si>
     <t xml:space="preserve">Torcy</t>
@@ -529,7 +535,7 @@
     <t xml:space="preserve">poorly sorted to well-sorted sandy gravel and gravely sand with silt and clay, alluvial terrace deposits</t>
   </si>
   <si>
-    <t xml:space="preserve">Adams and Gelhar, 1992, Bohling et al., 2016</t>
+    <t xml:space="preserve">Adams and Gelhar, 1992; Bohling et al., 2016</t>
   </si>
   <si>
     <t xml:space="preserve">Sum weights:</t>
@@ -541,7 +547,7 @@
     <t xml:space="preserve">WEIGHTED</t>
   </si>
   <si>
-    <t xml:space="preserve">Weight is N/K, with N=3,2,1 (high, medium, low information) and K=1,2 Reliability of AL (high, low)</t>
+    <t xml:space="preserve">Weight is k/R, with k=3,2,1 (high, medium, low information) and R=1,2 Reliability of AL (high, low)</t>
   </si>
   <si>
     <t xml:space="preserve">Low heterogeneity: prevalently sandy aquifers with some minor silt/clay or gravel</t>
@@ -553,18 +559,19 @@
     <t xml:space="preserve">High Heterogeneity: wide variety of materials, from gravel to clay, in similar %</t>
   </si>
   <si>
-    <t xml:space="preserve">NB: descriptions are rough and approximate!</t>
+    <t xml:space="preserve">Note: descriptions are rough and approximate!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -616,12 +623,54 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE994"/>
+        <bgColor rgb="FFFFDE59"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDE59"/>
+        <bgColor rgb="FFFFE994"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFFFF5CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA6A6"/>
+        <bgColor rgb="FFFFD7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7B59"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7B3CA"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -632,7 +681,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -726,7 +775,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="91">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -737,12 +786,20 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -751,28 +808,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -780,49 +845,205 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -851,11 +1072,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -863,43 +1084,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -907,26 +1128,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -944,14 +1165,14 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB7B3CA"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFF5CE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF7B59"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -965,15 +1186,15 @@
       <rgbColor rgb="FF00B0F0"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFFE994"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFA6A6"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF92D050"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFDE59"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -992,41 +1213,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G57" activeCellId="0" sqref="G57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R60" activeCellId="0" sqref="R60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="19" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="35" style="1" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1018" style="0" width="11.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="26.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="19" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="25" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="35" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1262,7 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1078,7 +1289,7 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
@@ -1114,75 +1325,82 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="4" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="s">
+    <row r="2" s="6" customFormat="true" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="N2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AMG2" s="6"/>
+      <c r="P2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="8"/>
+      <c r="AMG2" s="9"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="10" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="AMD3" s="11"/>
-      <c r="AME3" s="11"/>
-      <c r="AMF3" s="11"/>
-      <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="3" s="13" customFormat="true" ht="13.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>29</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="12"/>
+      <c r="AMD3" s="14"/>
+      <c r="AME3" s="14"/>
+      <c r="AMF3" s="14"/>
+      <c r="AMG3" s="15"/>
+      <c r="AMH3" s="15"/>
+      <c r="AMI3" s="15"/>
+      <c r="AMJ3" s="15"/>
+    </row>
+    <row r="4" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>50</v>
@@ -1218,16 +1436,16 @@
         <v>11</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="P4" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="R4" s="13" t="s">
-        <v>31</v>
+      <c r="R4" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="S4" s="1" t="n">
         <f aca="false">IF($P4=1,$C4,"")</f>
@@ -1254,9 +1472,9 @@
         <v/>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
+    <row r="5" customFormat="false" ht="48.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>90</v>
@@ -1295,16 +1513,16 @@
         <v>0.091</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P5" s="12" t="n">
+        <v>34</v>
+      </c>
+      <c r="P5" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="R5" s="1" t="s">
-        <v>34</v>
+      <c r="R5" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="S5" s="1" t="n">
         <f aca="false">IF($P5=1,$C5,"")</f>
@@ -1331,9 +1549,9 @@
         <v/>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>35</v>
+    <row r="6" customFormat="false" ht="48.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>200</v>
@@ -1375,16 +1593,16 @@
         <v>0.8</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="P6" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>37</v>
+      <c r="R6" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="S6" s="1" t="n">
         <f aca="false">IF($P6=1,$C6,"")</f>
@@ -1411,9 +1629,9 @@
         <v/>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>38</v>
+    <row r="7" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>212</v>
@@ -1452,16 +1670,16 @@
         <v>0.43</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P7" s="12" t="n">
+        <v>40</v>
+      </c>
+      <c r="P7" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="R7" s="1" t="s">
-        <v>40</v>
+      <c r="R7" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="S7" s="1" t="n">
         <f aca="false">IF($P7=1,$C7,"")</f>
@@ -1488,9 +1706,9 @@
         <v/>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
-        <v>41</v>
+    <row r="8" customFormat="false" ht="95.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>266</v>
@@ -1508,7 +1726,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>0.23</v>
@@ -1523,22 +1741,22 @@
         <v>0.032</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N8" s="1" t="n">
         <v>0.74</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" s="12" t="n">
+        <v>45</v>
+      </c>
+      <c r="P8" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="R8" s="1" t="s">
-        <v>45</v>
+      <c r="R8" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="S8" s="1" t="n">
         <f aca="false">IF($P8=1,$C8,"")</f>
@@ -1566,8 +1784,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="P9" s="12"/>
+      <c r="A9" s="6"/>
+      <c r="P9" s="16"/>
       <c r="S9" s="1" t="str">
         <f aca="false">IF($P9=1,$C9,"")</f>
         <v/>
@@ -1593,62 +1811,62 @@
         <v/>
       </c>
     </row>
-    <row r="10" s="16" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="1" t="str">
+    <row r="10" s="23" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="22" t="str">
         <f aca="false">IF($P10=1,$C10,"")</f>
         <v/>
       </c>
-      <c r="T10" s="1" t="str">
+      <c r="T10" s="22" t="str">
         <f aca="false">IF($P10=2,$C10,"")</f>
         <v/>
       </c>
-      <c r="U10" s="1" t="str">
+      <c r="U10" s="22" t="str">
         <f aca="false">IF($P10=3,$C10,"")</f>
         <v/>
       </c>
-      <c r="V10" s="1" t="str">
+      <c r="V10" s="22" t="str">
         <f aca="false">IF($P10=1,#REF!,"")</f>
         <v/>
       </c>
-      <c r="W10" s="1" t="str">
+      <c r="W10" s="22" t="str">
         <f aca="false">IF($P10=2,#REF!,"")</f>
         <v/>
       </c>
-      <c r="X10" s="1" t="str">
+      <c r="X10" s="22" t="str">
         <f aca="false">IF($P10=3,#REF!,"")</f>
         <v/>
       </c>
-      <c r="AMD10" s="17"/>
-      <c r="AME10" s="17"/>
-      <c r="AMF10" s="17"/>
-      <c r="AMG10" s="0"/>
-      <c r="AMH10" s="0"/>
-      <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>47</v>
+      <c r="AMD10" s="24"/>
+      <c r="AME10" s="24"/>
+      <c r="AMF10" s="24"/>
+      <c r="AMG10" s="25"/>
+      <c r="AMH10" s="25"/>
+      <c r="AMI10" s="25"/>
+      <c r="AMJ10" s="25"/>
+    </row>
+    <row r="11" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>52</v>
@@ -1681,16 +1899,16 @@
         <v>5.5</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P11" s="12" t="n">
+        <v>49</v>
+      </c>
+      <c r="P11" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="R11" s="1" t="s">
-        <v>49</v>
+      <c r="R11" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="S11" s="1" t="str">
         <f aca="false">IF($P11=1,$C11,"")</f>
@@ -1717,9 +1935,9 @@
         <v/>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>50</v>
+    <row r="12" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>170</v>
@@ -1758,16 +1976,16 @@
         <v>1.5</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P12" s="12" t="n">
+        <v>52</v>
+      </c>
+      <c r="P12" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q12" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="R12" s="1" t="s">
-        <v>52</v>
+      <c r="R12" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="S12" s="1" t="str">
         <f aca="false">IF($P12=1,$C12,"")</f>
@@ -1795,8 +2013,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="P13" s="12"/>
+      <c r="A13" s="6"/>
+      <c r="P13" s="16"/>
       <c r="S13" s="1" t="str">
         <f aca="false">IF($P13=1,$C13,"")</f>
         <v/>
@@ -1822,62 +2040,62 @@
         <v/>
       </c>
     </row>
-    <row r="14" s="16" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="1" t="str">
+    <row r="14" s="31" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="30" t="str">
         <f aca="false">IF($P14=1,$C14,"")</f>
         <v/>
       </c>
-      <c r="T14" s="1" t="str">
+      <c r="T14" s="30" t="str">
         <f aca="false">IF($P14=2,$C14,"")</f>
         <v/>
       </c>
-      <c r="U14" s="1" t="str">
+      <c r="U14" s="30" t="str">
         <f aca="false">IF($P14=3,$C14,"")</f>
         <v/>
       </c>
-      <c r="V14" s="1" t="str">
+      <c r="V14" s="30" t="str">
         <f aca="false">IF($P14=1,#REF!,"")</f>
         <v/>
       </c>
-      <c r="W14" s="1" t="str">
+      <c r="W14" s="30" t="str">
         <f aca="false">IF($P14=2,#REF!,"")</f>
         <v/>
       </c>
-      <c r="X14" s="1" t="str">
+      <c r="X14" s="30" t="str">
         <f aca="false">IF($P14=3,#REF!,"")</f>
         <v/>
       </c>
-      <c r="AMD14" s="17"/>
-      <c r="AME14" s="17"/>
-      <c r="AMF14" s="17"/>
-      <c r="AMG14" s="0"/>
-      <c r="AMH14" s="0"/>
-      <c r="AMI14" s="0"/>
-      <c r="AMJ14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>54</v>
+      <c r="AMD14" s="32"/>
+      <c r="AME14" s="32"/>
+      <c r="AMF14" s="32"/>
+      <c r="AMG14" s="33"/>
+      <c r="AMH14" s="33"/>
+      <c r="AMI14" s="33"/>
+      <c r="AMJ14" s="33"/>
+    </row>
+    <row r="15" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>52</v>
@@ -1895,10 +2113,10 @@
         <v>3.1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L15" s="1" t="n">
         <v>0.001</v>
@@ -1910,16 +2128,16 @@
         <v>3</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P15" s="12" t="n">
+        <v>58</v>
+      </c>
+      <c r="P15" s="16" t="n">
         <v>3</v>
       </c>
       <c r="Q15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="R15" s="1" t="s">
-        <v>58</v>
+      <c r="R15" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="S15" s="1" t="str">
         <f aca="false">IF($P15=1,$C15,"")</f>
@@ -1947,7 +2165,6 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
       <c r="D16" s="0"/>
@@ -1961,10 +2178,8 @@
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
       <c r="N16" s="0"/>
-      <c r="O16" s="0"/>
-      <c r="P16" s="6"/>
+      <c r="P16" s="9"/>
       <c r="Q16" s="0"/>
-      <c r="R16" s="0"/>
       <c r="S16" s="0"/>
       <c r="T16" s="0"/>
       <c r="U16" s="0"/>
@@ -2965,62 +3180,62 @@
       <c r="AMB16" s="0"/>
       <c r="AMC16" s="0"/>
     </row>
-    <row r="17" s="16" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="1" t="str">
+    <row r="17" s="39" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="38" t="str">
         <f aca="false">IF($P17=1,$C17,"")</f>
         <v/>
       </c>
-      <c r="T17" s="1" t="str">
+      <c r="T17" s="38" t="str">
         <f aca="false">IF($P17=2,$C17,"")</f>
         <v/>
       </c>
-      <c r="U17" s="1" t="str">
+      <c r="U17" s="38" t="str">
         <f aca="false">IF($P17=3,$C17,"")</f>
         <v/>
       </c>
-      <c r="V17" s="1" t="str">
+      <c r="V17" s="38" t="str">
         <f aca="false">IF($P17=1,#REF!,"")</f>
         <v/>
       </c>
-      <c r="W17" s="1" t="str">
+      <c r="W17" s="38" t="str">
         <f aca="false">IF($P17=2,#REF!,"")</f>
         <v/>
       </c>
-      <c r="X17" s="1" t="str">
+      <c r="X17" s="38" t="str">
         <f aca="false">IF($P17=3,#REF!,"")</f>
         <v/>
       </c>
-      <c r="AMD17" s="17"/>
-      <c r="AME17" s="17"/>
-      <c r="AMF17" s="17"/>
-      <c r="AMG17" s="0"/>
-      <c r="AMH17" s="0"/>
-      <c r="AMI17" s="0"/>
-      <c r="AMJ17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>60</v>
+      <c r="AMD17" s="40"/>
+      <c r="AME17" s="40"/>
+      <c r="AMF17" s="40"/>
+      <c r="AMG17" s="41"/>
+      <c r="AMH17" s="41"/>
+      <c r="AMI17" s="41"/>
+      <c r="AMJ17" s="41"/>
+    </row>
+    <row r="18" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>16</v>
@@ -3044,16 +3259,16 @@
         <v>27</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P18" s="12" t="n">
+        <v>62</v>
+      </c>
+      <c r="P18" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q18" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R18" s="1" t="s">
-        <v>62</v>
+      <c r="R18" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="S18" s="1" t="n">
         <f aca="false">IF($P18=1,$C18,"")</f>
@@ -3080,9 +3295,9 @@
         <v/>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>63</v>
+    <row r="19" customFormat="false" ht="60.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>18.3</v>
@@ -3109,16 +3324,16 @@
         <v>29</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P19" s="12" t="n">
+        <v>65</v>
+      </c>
+      <c r="P19" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q19" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R19" s="1" t="s">
-        <v>65</v>
+      <c r="R19" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="S19" s="1" t="n">
         <f aca="false">IF($P19=1,$C19,"")</f>
@@ -3145,9 +3360,9 @@
         <v/>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>66</v>
+    <row r="20" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>25</v>
@@ -3165,16 +3380,16 @@
         <v>0.42</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P20" s="12" t="n">
+        <v>68</v>
+      </c>
+      <c r="P20" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q20" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R20" s="1" t="s">
-        <v>68</v>
+      <c r="R20" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="S20" s="1" t="n">
         <f aca="false">IF($P20=1,$C20,"")</f>
@@ -3201,9 +3416,9 @@
         <v/>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>69</v>
+    <row r="21" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>32.5</v>
@@ -3227,16 +3442,16 @@
         <v>1.9</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="P21" s="12" t="n">
+        <v>71</v>
+      </c>
+      <c r="P21" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q21" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R21" s="1" t="s">
-        <v>71</v>
+      <c r="R21" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="S21" s="1" t="n">
         <f aca="false">IF($P21=1,$C21,"")</f>
@@ -3263,9 +3478,9 @@
         <v/>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>72</v>
+    <row r="22" customFormat="false" ht="72.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>38.3</v>
@@ -3280,7 +3495,7 @@
         <v>0.615</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L22" s="1" t="n">
         <v>0.00033</v>
@@ -3292,16 +3507,16 @@
         <v>0.05</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P22" s="12" t="n">
+        <v>75</v>
+      </c>
+      <c r="P22" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q22" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R22" s="1" t="s">
-        <v>75</v>
+      <c r="R22" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="S22" s="1" t="n">
         <f aca="false">IF($P22=1,$C22,"")</f>
@@ -3328,9 +3543,9 @@
         <v/>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>76</v>
+    <row r="23" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>50</v>
@@ -3362,17 +3577,17 @@
       <c r="N23" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="P23" s="12" t="n">
+      <c r="O23" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="P23" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R23" s="1" t="s">
-        <v>78</v>
+      <c r="R23" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="S23" s="1" t="n">
         <f aca="false">IF($P23=1,$C23,"")</f>
@@ -3398,9 +3613,9 @@
         <v/>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>79</v>
+    <row r="24" customFormat="false" ht="72.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>130</v>
@@ -3436,16 +3651,16 @@
         <v>0.11</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="P24" s="12" t="n">
+        <v>81</v>
+      </c>
+      <c r="P24" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q24" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R24" s="1" t="s">
-        <v>81</v>
+      <c r="R24" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="S24" s="1" t="n">
         <f aca="false">IF($P24=1,$C24,"")</f>
@@ -3472,9 +3687,9 @@
         <v/>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>82</v>
+    <row r="25" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>350</v>
@@ -3498,16 +3713,16 @@
         <v>9.14</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="P25" s="12" t="n">
+        <v>84</v>
+      </c>
+      <c r="P25" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q25" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="R25" s="1" t="s">
-        <v>84</v>
+      <c r="R25" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="S25" s="1" t="n">
         <f aca="false">IF($P25=1,$C25,"")</f>
@@ -3534,9 +3749,9 @@
         <v/>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>85</v>
+    <row r="26" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>1000</v>
@@ -3548,7 +3763,7 @@
         <v>2</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K26" s="1" t="n">
         <v>0.35</v>
@@ -3557,16 +3772,16 @@
         <v>40</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="P26" s="12" t="n">
+        <v>88</v>
+      </c>
+      <c r="P26" s="16" t="n">
         <v>1</v>
       </c>
       <c r="Q26" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R26" s="1" t="s">
-        <v>88</v>
+      <c r="R26" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="S26" s="1" t="n">
         <f aca="false">IF($P26=1,$C26,"")</f>
@@ -3594,8 +3809,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4"/>
-      <c r="P27" s="12"/>
+      <c r="A27" s="6"/>
+      <c r="P27" s="16"/>
       <c r="S27" s="1" t="str">
         <f aca="false">IF($P27=1,$C27,"")</f>
         <v/>
@@ -3621,62 +3836,62 @@
         <v/>
       </c>
     </row>
-    <row r="28" s="16" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="1" t="str">
+    <row r="28" s="47" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="44"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="46" t="str">
         <f aca="false">IF($P28=1,$C28,"")</f>
         <v/>
       </c>
-      <c r="T28" s="1" t="str">
+      <c r="T28" s="46" t="str">
         <f aca="false">IF($P28=2,$C28,"")</f>
         <v/>
       </c>
-      <c r="U28" s="1" t="str">
+      <c r="U28" s="46" t="str">
         <f aca="false">IF($P28=3,$C28,"")</f>
         <v/>
       </c>
-      <c r="V28" s="1" t="str">
+      <c r="V28" s="46" t="str">
         <f aca="false">IF($P28=1,#REF!,"")</f>
         <v/>
       </c>
-      <c r="W28" s="1" t="str">
+      <c r="W28" s="46" t="str">
         <f aca="false">IF($P28=2,#REF!,"")</f>
         <v/>
       </c>
-      <c r="X28" s="1" t="str">
+      <c r="X28" s="46" t="str">
         <f aca="false">IF($P28=3,#REF!,"")</f>
         <v/>
       </c>
-      <c r="AMD28" s="17"/>
-      <c r="AME28" s="17"/>
-      <c r="AMF28" s="17"/>
-      <c r="AMG28" s="0"/>
-      <c r="AMH28" s="0"/>
-      <c r="AMI28" s="0"/>
-      <c r="AMJ28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>89</v>
+      <c r="AMD28" s="48"/>
+      <c r="AME28" s="48"/>
+      <c r="AMF28" s="48"/>
+      <c r="AMG28" s="49"/>
+      <c r="AMH28" s="49"/>
+      <c r="AMI28" s="49"/>
+      <c r="AMJ28" s="49"/>
+    </row>
+    <row r="29" customFormat="false" ht="48.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>15.5</v>
@@ -3700,16 +3915,16 @@
         <v>13.2</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="P29" s="12" t="n">
+        <v>92</v>
+      </c>
+      <c r="P29" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q29" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R29" s="1" t="s">
-        <v>91</v>
+      <c r="R29" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="S29" s="1" t="str">
         <f aca="false">IF($P29=1,$C29,"")</f>
@@ -3736,9 +3951,9 @@
         <v/>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>92</v>
+    <row r="30" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>19</v>
@@ -3762,16 +3977,16 @@
         <v>7</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="P30" s="12" t="n">
+        <v>95</v>
+      </c>
+      <c r="P30" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q30" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R30" s="1" t="s">
-        <v>94</v>
+      <c r="R30" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="S30" s="1" t="str">
         <f aca="false">IF($P30=1,$C30,"")</f>
@@ -3798,9 +4013,9 @@
         <v/>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>95</v>
+    <row r="31" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>40</v>
@@ -3827,16 +4042,16 @@
         <v>0.05</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="P31" s="12" t="n">
+        <v>98</v>
+      </c>
+      <c r="P31" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="R31" s="1" t="s">
-        <v>97</v>
+      <c r="R31" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="S31" s="1" t="str">
         <f aca="false">IF($P31=1,$C31,"")</f>
@@ -3863,9 +4078,9 @@
         <v/>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>98</v>
+    <row r="32" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>55</v>
@@ -3892,16 +4107,16 @@
         <v>0.5</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P32" s="12" t="n">
+        <v>101</v>
+      </c>
+      <c r="P32" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q32" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R32" s="1" t="s">
-        <v>100</v>
+      <c r="R32" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="S32" s="0"/>
       <c r="T32" s="1" t="n">
@@ -3921,9 +4136,9 @@
         <v/>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
-        <v>101</v>
+    <row r="33" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>79.3</v>
@@ -3941,16 +4156,16 @@
         <v>10.5</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="P33" s="12" t="n">
+        <v>104</v>
+      </c>
+      <c r="P33" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q33" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R33" s="1" t="s">
-        <v>103</v>
+      <c r="R33" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="S33" s="1" t="str">
         <f aca="false">IF($P33=1,$C33,"")</f>
@@ -3977,9 +4192,9 @@
         <v/>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
-        <v>104</v>
+    <row r="34" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>80</v>
@@ -4003,16 +4218,16 @@
         <v>3.5</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="P34" s="12" t="n">
+        <v>107</v>
+      </c>
+      <c r="P34" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q34" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R34" s="1" t="s">
-        <v>106</v>
+      <c r="R34" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="S34" s="1" t="str">
         <f aca="false">IF($P34=1,$C34,"")</f>
@@ -4039,9 +4254,9 @@
         <v/>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
-        <v>107</v>
+    <row r="35" customFormat="false" ht="72.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>87</v>
@@ -4065,16 +4280,16 @@
         <v>60</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="P35" s="12" t="n">
+        <v>110</v>
+      </c>
+      <c r="P35" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q35" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R35" s="1" t="s">
-        <v>109</v>
+      <c r="R35" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="S35" s="1" t="str">
         <f aca="false">IF($P35=1,$C35,"")</f>
@@ -4101,9 +4316,9 @@
         <v/>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>110</v>
+    <row r="36" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>164</v>
@@ -4115,7 +4330,7 @@
         <v>2</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="L36" s="1" t="n">
         <v>0.006</v>
@@ -4124,16 +4339,16 @@
         <v>27</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="P36" s="12" t="n">
+        <v>114</v>
+      </c>
+      <c r="P36" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q36" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="R36" s="1" t="s">
-        <v>113</v>
+      <c r="R36" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="S36" s="1" t="str">
         <f aca="false">IF($P36=1,$C36,"")</f>
@@ -4160,16 +4375,13 @@
         <v/>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>114</v>
+    <row r="37" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="D37" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="F37" s="1" t="n">
         <v>0.032</v>
       </c>
@@ -4186,16 +4398,16 @@
         <v>2.7</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="P37" s="12" t="n">
+        <v>117</v>
+      </c>
+      <c r="P37" s="16" t="n">
         <v>2</v>
       </c>
       <c r="Q37" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R37" s="1" t="s">
-        <v>116</v>
+      <c r="R37" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="S37" s="1" t="str">
         <f aca="false">IF($P37=1,$C37,"")</f>
@@ -4223,61 +4435,61 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6"/>
-      <c r="P38" s="19"/>
-    </row>
-    <row r="39" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="20"/>
-      <c r="S39" s="1" t="str">
+      <c r="P38" s="50"/>
+    </row>
+    <row r="39" s="56" customFormat="true" ht="13.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="52"/>
+      <c r="M39" s="52"/>
+      <c r="N39" s="52"/>
+      <c r="O39" s="53"/>
+      <c r="P39" s="54"/>
+      <c r="Q39" s="52"/>
+      <c r="R39" s="53"/>
+      <c r="S39" s="55" t="str">
         <f aca="false">IF($P39=1,$C39,"")</f>
         <v/>
       </c>
-      <c r="T39" s="1" t="str">
+      <c r="T39" s="55" t="str">
         <f aca="false">IF($P39=2,$C39,"")</f>
         <v/>
       </c>
-      <c r="U39" s="1" t="str">
+      <c r="U39" s="55" t="str">
         <f aca="false">IF($P39=3,$C39,"")</f>
         <v/>
       </c>
-      <c r="V39" s="1" t="str">
+      <c r="V39" s="55" t="str">
         <f aca="false">IF($P39=1,#REF!,"")</f>
         <v/>
       </c>
-      <c r="W39" s="1" t="str">
+      <c r="W39" s="55" t="str">
         <f aca="false">IF($P39=2,#REF!,"")</f>
         <v/>
       </c>
-      <c r="X39" s="1" t="str">
+      <c r="X39" s="55" t="str">
         <f aca="false">IF($P39=3,#REF!,"")</f>
         <v/>
       </c>
-      <c r="AMG39" s="0"/>
-      <c r="AMH39" s="0"/>
-      <c r="AMI39" s="0"/>
-      <c r="AMJ39" s="0"/>
-    </row>
-    <row r="40" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
-        <v>118</v>
+      <c r="AMG39" s="57"/>
+      <c r="AMH39" s="57"/>
+      <c r="AMI39" s="57"/>
+      <c r="AMJ39" s="57"/>
+    </row>
+    <row r="40" customFormat="false" ht="72.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>15</v>
@@ -4301,16 +4513,16 @@
         <v>11</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="P40" s="12" t="n">
+        <v>121</v>
+      </c>
+      <c r="P40" s="16" t="n">
         <v>3</v>
       </c>
       <c r="Q40" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R40" s="1" t="s">
-        <v>120</v>
+      <c r="R40" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="S40" s="1" t="str">
         <f aca="false">IF($P40=1,$C40,"")</f>
@@ -4337,9 +4549,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>121</v>
+    <row r="41" customFormat="false" ht="48.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>45</v>
@@ -4372,16 +4584,16 @@
         <v>15</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="P41" s="12" t="n">
+        <v>124</v>
+      </c>
+      <c r="P41" s="16" t="n">
         <v>3</v>
       </c>
       <c r="Q41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R41" s="1" t="s">
-        <v>123</v>
+      <c r="R41" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="S41" s="1" t="str">
         <f aca="false">IF($P41=1,$C41,"")</f>
@@ -4408,9 +4620,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>124</v>
+    <row r="42" customFormat="false" ht="72.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>57</v>
@@ -4440,16 +4652,16 @@
         <v>145</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="P42" s="12" t="n">
+        <v>127</v>
+      </c>
+      <c r="P42" s="16" t="n">
         <v>3</v>
       </c>
       <c r="Q42" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R42" s="1" t="s">
-        <v>126</v>
+      <c r="R42" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="S42" s="1" t="str">
         <f aca="false">IF($P42=1,$C42,"")</f>
@@ -4476,9 +4688,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
-        <v>127</v>
+    <row r="43" customFormat="false" ht="72.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>110</v>
@@ -4496,7 +4708,7 @@
         <v>2.15</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K43" s="1" t="n">
         <v>0.25</v>
@@ -4511,16 +4723,16 @@
         <v>3</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="P43" s="12" t="n">
+        <v>131</v>
+      </c>
+      <c r="P43" s="16" t="n">
         <v>3</v>
       </c>
       <c r="Q43" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R43" s="1" t="s">
-        <v>130</v>
+      <c r="R43" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="S43" s="1" t="str">
         <f aca="false">IF($P43=1,$C43,"")</f>
@@ -4547,9 +4759,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>131</v>
+    <row r="44" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>150</v>
@@ -4564,16 +4776,16 @@
         <v>12</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="P44" s="12" t="n">
+        <v>134</v>
+      </c>
+      <c r="P44" s="16" t="n">
         <v>3</v>
       </c>
       <c r="Q44" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="R44" s="1" t="s">
-        <v>133</v>
+      <c r="R44" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="S44" s="1" t="str">
         <f aca="false">IF($P44=1,$C44,"")</f>
@@ -4600,9 +4812,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>134</v>
+    <row r="45" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>3500</v>
@@ -4626,16 +4838,16 @@
         <v>26</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="P45" s="12" t="n">
+        <v>137</v>
+      </c>
+      <c r="P45" s="16" t="n">
         <v>3</v>
       </c>
       <c r="Q45" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R45" s="1" t="s">
-        <v>136</v>
+      <c r="R45" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="S45" s="1" t="str">
         <f aca="false">IF($P45=1,$C45,"")</f>
@@ -4663,64 +4875,64 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P46" s="23"/>
-    </row>
-    <row r="47" s="16" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="1" t="str">
+      <c r="P46" s="58"/>
+    </row>
+    <row r="47" s="64" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="60"/>
+      <c r="K47" s="60"/>
+      <c r="L47" s="60"/>
+      <c r="M47" s="60"/>
+      <c r="N47" s="60"/>
+      <c r="O47" s="60"/>
+      <c r="P47" s="61"/>
+      <c r="Q47" s="60"/>
+      <c r="R47" s="62"/>
+      <c r="S47" s="63" t="str">
         <f aca="false">IF($P47=1,$C47,"")</f>
         <v/>
       </c>
-      <c r="T47" s="1" t="str">
+      <c r="T47" s="63" t="str">
         <f aca="false">IF($P47=2,$C47,"")</f>
         <v/>
       </c>
-      <c r="U47" s="1" t="str">
+      <c r="U47" s="63" t="str">
         <f aca="false">IF($P47=3,$C47,"")</f>
         <v/>
       </c>
-      <c r="V47" s="1" t="str">
+      <c r="V47" s="63" t="str">
         <f aca="false">IF($P47=1,#REF!,"")</f>
         <v/>
       </c>
-      <c r="W47" s="1" t="str">
+      <c r="W47" s="63" t="str">
         <f aca="false">IF($P47=2,#REF!,"")</f>
         <v/>
       </c>
-      <c r="X47" s="1" t="str">
+      <c r="X47" s="63" t="str">
         <f aca="false">IF($P47=3,#REF!,"")</f>
         <v/>
       </c>
-      <c r="AMD47" s="17"/>
-      <c r="AME47" s="17"/>
-      <c r="AMF47" s="17"/>
-      <c r="AMG47" s="0"/>
-      <c r="AMH47" s="0"/>
-      <c r="AMI47" s="0"/>
-      <c r="AMJ47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMD47" s="65"/>
+      <c r="AME47" s="65"/>
+      <c r="AMF47" s="65"/>
+      <c r="AMG47" s="66"/>
+      <c r="AMH47" s="66"/>
+      <c r="AMI47" s="66"/>
+      <c r="AMJ47" s="66"/>
+    </row>
+    <row r="48" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>4.5</v>
@@ -4747,14 +4959,14 @@
         <v>0.72</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P48" s="24"/>
+        <v>141</v>
+      </c>
+      <c r="P48" s="67"/>
       <c r="Q48" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R48" s="1" t="s">
-        <v>140</v>
+      <c r="R48" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="S48" s="1" t="str">
         <f aca="false">IF($P48=1,$C48,"")</f>
@@ -4780,9 +4992,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>5.2</v>
@@ -4803,14 +5015,14 @@
         <v>9</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="P49" s="24"/>
+        <v>144</v>
+      </c>
+      <c r="P49" s="67"/>
       <c r="Q49" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R49" s="1" t="s">
-        <v>143</v>
+      <c r="R49" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="S49" s="1" t="str">
         <f aca="false">IF($P49=1,$C49,"")</f>
@@ -4836,9 +5048,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>5.5</v>
@@ -4862,14 +5074,14 @@
         <v>29</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="P50" s="24"/>
+        <v>147</v>
+      </c>
+      <c r="P50" s="67"/>
       <c r="Q50" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R50" s="1" t="s">
-        <v>146</v>
+      <c r="R50" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="S50" s="1" t="str">
         <f aca="false">IF($P50=1,$C50,"")</f>
@@ -4897,7 +5109,7 @@
     </row>
     <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>6.5</v>
@@ -4912,14 +5124,14 @@
         <v>10</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="P51" s="24"/>
+        <v>150</v>
+      </c>
+      <c r="P51" s="67"/>
       <c r="Q51" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R51" s="1" t="s">
-        <v>149</v>
+      <c r="R51" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="S51" s="1" t="str">
         <f aca="false">IF($P51=1,$C51,"")</f>
@@ -4945,9 +5157,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>7.1</v>
@@ -4971,14 +5183,14 @@
         <v>18</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="P52" s="24"/>
+        <v>153</v>
+      </c>
+      <c r="P52" s="67"/>
       <c r="Q52" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R52" s="1" t="s">
-        <v>152</v>
+      <c r="R52" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="S52" s="1" t="str">
         <f aca="false">IF($P52=1,$C52,"")</f>
@@ -5004,9 +5216,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B53" s="1" t="n">
         <v>8</v>
@@ -5024,14 +5236,14 @@
         <v>0.12</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="P53" s="24"/>
+        <v>156</v>
+      </c>
+      <c r="P53" s="67"/>
       <c r="Q53" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R53" s="1" t="s">
-        <v>155</v>
+      <c r="R53" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="S53" s="1" t="str">
         <f aca="false">IF($P53=1,$C53,"")</f>
@@ -5057,9 +5269,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B54" s="1" t="n">
         <v>10</v>
@@ -5077,14 +5289,14 @@
         <v>20</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="P54" s="24"/>
+        <v>159</v>
+      </c>
+      <c r="P54" s="67"/>
       <c r="Q54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R54" s="1" t="s">
-        <v>158</v>
+      <c r="R54" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="S54" s="1" t="str">
         <f aca="false">IF($P54=1,$C54,"")</f>
@@ -5110,9 +5322,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B55" s="1" t="n">
         <v>13.8</v>
@@ -5130,14 +5342,14 @@
         <v>19</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P55" s="24"/>
+        <v>162</v>
+      </c>
+      <c r="P55" s="67"/>
       <c r="Q55" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R55" s="1" t="s">
-        <v>161</v>
+      <c r="R55" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="S55" s="1" t="str">
         <f aca="false">IF($P55=1,$C55,"")</f>
@@ -5163,9 +5375,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B56" s="1" t="n">
         <v>15</v>
@@ -5186,14 +5398,14 @@
         <v>0.5</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P56" s="24"/>
+        <v>52</v>
+      </c>
+      <c r="P56" s="67"/>
       <c r="Q56" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R56" s="1" t="s">
-        <v>163</v>
+      <c r="R56" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="S56" s="1" t="str">
         <f aca="false">IF($P56=1,$C56,"")</f>
@@ -5219,9 +5431,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
-        <v>164</v>
+    <row r="57" customFormat="false" ht="48.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="B57" s="1" t="n">
         <v>200</v>
@@ -5236,10 +5448,10 @@
         <v>0.0067</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K57" s="1" t="n">
         <v>0.32</v>
@@ -5251,17 +5463,17 @@
         <v>8</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="P57" s="24"/>
+        <v>170</v>
+      </c>
+      <c r="P57" s="67"/>
       <c r="Q57" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="R57" s="1" t="s">
-        <v>169</v>
+      <c r="R57" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="S57" s="1" t="str">
         <f aca="false">IF($P57=1,$C57,"")</f>
@@ -5288,7 +5500,6 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0"/>
       <c r="B58" s="0"/>
       <c r="C58" s="0"/>
       <c r="D58" s="0"/>
@@ -5302,10 +5513,8 @@
       <c r="L58" s="0"/>
       <c r="M58" s="0"/>
       <c r="N58" s="0"/>
-      <c r="O58" s="0"/>
       <c r="P58" s="0"/>
       <c r="Q58" s="0"/>
-      <c r="R58" s="0"/>
       <c r="S58" s="0"/>
       <c r="T58" s="0"/>
       <c r="U58" s="0"/>
@@ -6306,9 +6515,9 @@
       <c r="AMB58" s="0"/>
       <c r="AMC58" s="0"/>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="U62" s="25" t="s">
-        <v>170</v>
+    <row r="62" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U62" s="68" t="s">
+        <v>172</v>
       </c>
       <c r="V62" s="1" t="n">
         <f aca="false">SUM(V4:V61)</f>
@@ -6324,177 +6533,176 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="U63" s="25"/>
+      <c r="U63" s="68"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R64" s="0"/>
-      <c r="S64" s="26"/>
-      <c r="T64" s="27" t="s">
+      <c r="S64" s="69"/>
+      <c r="T64" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="U64" s="27" t="s">
+      <c r="U64" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="V64" s="28" t="s">
+      <c r="V64" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="W64" s="29"/>
-    </row>
-    <row r="65" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R65" s="0"/>
-      <c r="S65" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="T65" s="31" t="n">
+      <c r="W64" s="72"/>
+    </row>
+    <row r="65" customFormat="false" ht="39.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S65" s="73" t="s">
+        <v>173</v>
+      </c>
+      <c r="T65" s="74" t="n">
         <f aca="false">COUNTIF(S4:S61,"&gt;0")</f>
         <v>13</v>
       </c>
-      <c r="U65" s="31" t="n">
+      <c r="U65" s="74" t="n">
         <f aca="false">COUNTIF(T4:T61,"&gt;0")</f>
         <v>10</v>
       </c>
-      <c r="V65" s="32" t="n">
+      <c r="V65" s="75" t="n">
         <f aca="false">COUNTIF(U4:U61,"&gt;0")</f>
         <v>7</v>
       </c>
-      <c r="W65" s="29"/>
-    </row>
-    <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R66" s="0"/>
-      <c r="S66" s="33"/>
-      <c r="T66" s="34" t="n">
+      <c r="W65" s="72"/>
+    </row>
+    <row r="66" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S66" s="76"/>
+      <c r="T66" s="77" t="n">
         <f aca="false">AVERAGEIF(S4:S61,"&gt;0")</f>
         <v>1.16230769230769</v>
       </c>
-      <c r="U66" s="34" t="n">
+      <c r="U66" s="77" t="n">
         <f aca="false">AVERAGEIF(T4:T61,"&gt;0")</f>
         <v>3.045</v>
       </c>
-      <c r="V66" s="35" t="n">
+      <c r="V66" s="78" t="n">
         <f aca="false">AVERAGEIF(U4:U61,"&gt;0")</f>
         <v>7.46857142857143</v>
       </c>
-      <c r="W66" s="29"/>
-    </row>
-    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R67" s="0"/>
-      <c r="S67" s="33"/>
-      <c r="T67" s="34" t="n">
+      <c r="W66" s="72"/>
+    </row>
+    <row r="67" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S67" s="76"/>
+      <c r="T67" s="77" t="n">
         <f aca="false">_xlfn.STDEV.S(S4:S61)</f>
         <v>1.07454079126291</v>
       </c>
-      <c r="U67" s="34" t="n">
+      <c r="U67" s="77" t="n">
         <f aca="false">_xlfn.STDEV.S(T4:T61)</f>
         <v>1.73576967470813</v>
       </c>
-      <c r="V67" s="35" t="n">
+      <c r="V67" s="78" t="n">
         <f aca="false">_xlfn.STDEV.S(U4:U61)</f>
         <v>3.05727236040793</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R68" s="0"/>
-      <c r="S68" s="33"/>
-      <c r="T68" s="34" t="n">
+    <row r="68" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S68" s="76"/>
+      <c r="T68" s="77" t="n">
         <f aca="false">T67/T66</f>
         <v>0.924489099034929</v>
       </c>
-      <c r="U68" s="34" t="n">
+      <c r="U68" s="77" t="n">
         <f aca="false">U67/U66</f>
         <v>0.570039302038794</v>
       </c>
-      <c r="V68" s="35" t="n">
+      <c r="V68" s="78" t="n">
         <f aca="false">V67/V66</f>
         <v>0.409351693245132</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R69" s="0"/>
-      <c r="S69" s="33"/>
-      <c r="T69" s="34"/>
-      <c r="U69" s="34"/>
-      <c r="V69" s="35"/>
-    </row>
-    <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R70" s="0"/>
-      <c r="S70" s="36" t="s">
-        <v>172</v>
-      </c>
-      <c r="T70" s="37" t="n">
+      <c r="S69" s="76"/>
+      <c r="T69" s="77"/>
+      <c r="U69" s="77"/>
+      <c r="V69" s="78"/>
+    </row>
+    <row r="70" customFormat="false" ht="26.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S70" s="79" t="s">
+        <v>174</v>
+      </c>
+      <c r="T70" s="80" t="n">
         <f aca="false">SUMPRODUCT(S4:S61,V4:V61)/V62</f>
         <v>1.14479166666667</v>
       </c>
-      <c r="U70" s="38" t="n">
+      <c r="U70" s="81" t="n">
         <f aca="false">SUMPRODUCT(T4:T61,W4:W61)/W62</f>
         <v>3.2076</v>
       </c>
-      <c r="V70" s="39" t="n">
+      <c r="V70" s="82" t="n">
         <f aca="false">SUMPRODUCT(U4:U61,X4:X61)/X62</f>
         <v>7.50428571428571</v>
       </c>
-      <c r="W70" s="40"/>
-      <c r="X70" s="40"/>
-    </row>
-    <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R71" s="0"/>
-      <c r="S71" s="33"/>
-      <c r="T71" s="41" t="n">
+      <c r="W70" s="83"/>
+      <c r="X70" s="83"/>
+    </row>
+    <row r="71" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S71" s="76"/>
+      <c r="T71" s="84" t="n">
         <f aca="false">SQRT(SUMPRODUCT(S4:S61,S4:S61,V4:V61)/V62-T70^2)</f>
         <v>1.06517602141488</v>
       </c>
-      <c r="U71" s="42" t="n">
+      <c r="U71" s="85" t="n">
         <f aca="false">SQRT(SUMPRODUCT(T4:T61,T4:T61,W4:W61)/W62-U70^2)</f>
         <v>1.49670111912833</v>
       </c>
-      <c r="V71" s="43" t="n">
+      <c r="V71" s="86" t="n">
         <f aca="false">SQRT(SUMPRODUCT(U4:U61,U4:U61,X4:X61)/X62-V70^2)</f>
         <v>2.87136780319493</v>
       </c>
-      <c r="W71" s="40"/>
-      <c r="X71" s="40"/>
-    </row>
-    <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R72" s="0"/>
-      <c r="S72" s="44"/>
-      <c r="T72" s="45" t="n">
+      <c r="W71" s="83"/>
+      <c r="X71" s="83"/>
+    </row>
+    <row r="72" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S72" s="87"/>
+      <c r="T72" s="88" t="n">
         <f aca="false">T71/T70</f>
         <v>0.930454031445205</v>
       </c>
-      <c r="U72" s="46" t="n">
+      <c r="U72" s="89" t="n">
         <f aca="false">U71/U70</f>
-        <v>0.466610898842851</v>
-      </c>
-      <c r="V72" s="47" t="n">
+        <v>0.466610898842852</v>
+      </c>
+      <c r="V72" s="90" t="n">
         <f aca="false">V71/V70</f>
         <v>0.382630394486284</v>
       </c>
-      <c r="W72" s="40"/>
-      <c r="X72" s="40"/>
-    </row>
-    <row r="73" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R73" s="0"/>
+      <c r="W72" s="83"/>
+      <c r="X72" s="83"/>
+    </row>
+    <row r="73" customFormat="false" ht="119.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S73" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="T73" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="U73" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="V73" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="72.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T74" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A47:F47"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="80" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="80" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>